<commit_message>
eg3 1-56 65-136 145-264
</commit_message>
<xml_diff>
--- a/eg3.xlsx
+++ b/eg3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shiqing/Desktop/Lipschitz-System-ID/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB8B31EC-462F-314B-BB3A-7CCE02860F7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23E73DE7-B414-D64F-B0CA-512C12676327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="820" windowWidth="34560" windowHeight="19800" activeTab="5" xr2:uid="{624D5C9E-D399-6E42-9BAD-9829FF00FD61}"/>
+    <workbookView xWindow="13180" yWindow="3600" windowWidth="34560" windowHeight="19800" activeTab="5" xr2:uid="{624D5C9E-D399-6E42-9BAD-9829FF00FD61}"/>
   </bookViews>
   <sheets>
     <sheet name="Ours 0.25" sheetId="1" r:id="rId1"/>
@@ -2098,15 +2098,15 @@
       </c>
       <c r="K4" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.98883008956909102</v>
+        <v>1.2735849618911701</v>
       </c>
       <c r="L4" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>1.6530596564213376E-3</v>
+        <v>2.6970230384419352E-3</v>
       </c>
       <c r="M4" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>1.6510131919974425E-3</v>
+        <v>2.6938984197802151E-3</v>
       </c>
       <c r="N4" s="4">
         <f t="shared" ca="1" si="0"/>
@@ -2142,15 +2142,15 @@
       </c>
       <c r="K5" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.97766017913818</v>
+        <v>2.5471699237823402</v>
       </c>
       <c r="L5" s="7">
         <f t="shared" ca="1" si="0"/>
-        <v>1.6381777262625575E-3</v>
+        <v>2.6745605363200052E-3</v>
       </c>
       <c r="M5" s="7">
         <f t="shared" ca="1" si="0"/>
-        <v>1.641923219877035E-3</v>
+        <v>2.6806525717628076E-3</v>
       </c>
       <c r="N5" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -2300,13 +2300,13 @@
         <v>2</v>
       </c>
       <c r="B10" s="4">
-        <v>0.98883008956909102</v>
+        <v>1.2735849618911701</v>
       </c>
       <c r="C10" s="6">
-        <v>1.6515019355962601E-3</v>
+        <v>2.6950021479278802E-3</v>
       </c>
       <c r="D10" s="6">
-        <v>1.65470736348961E-3</v>
+        <v>2.7023559148879098E-3</v>
       </c>
       <c r="E10" s="4">
         <v>57</v>
@@ -2320,13 +2320,13 @@
         <v>2</v>
       </c>
       <c r="B11" s="4">
-        <v>0.98883008956909102</v>
+        <v>1.2735849618911701</v>
       </c>
       <c r="C11" s="6">
-        <v>1.65478420692185E-3</v>
+        <v>2.6946473425875101E-3</v>
       </c>
       <c r="D11" s="6">
-        <v>1.6488772594033E-3</v>
+        <v>2.6820493599479102E-3</v>
       </c>
       <c r="E11" s="4">
         <v>58</v>
@@ -2340,13 +2340,13 @@
         <v>2</v>
       </c>
       <c r="B12" s="4">
-        <v>0.98883008956909102</v>
+        <v>1.2735849618911701</v>
       </c>
       <c r="C12" s="6">
-        <v>1.65669161826372E-3</v>
+        <v>2.7022943900277198E-3</v>
       </c>
       <c r="D12" s="6">
-        <v>1.64585960583087E-3</v>
+        <v>2.6868357932432799E-3</v>
       </c>
       <c r="E12" s="4">
         <v>59</v>
@@ -2360,13 +2360,13 @@
         <v>2</v>
       </c>
       <c r="B13" s="4">
-        <v>0.98883008956909102</v>
+        <v>1.2735849618911701</v>
       </c>
       <c r="C13" s="6">
-        <v>1.6492608649035199E-3</v>
+        <v>2.6961482732246302E-3</v>
       </c>
       <c r="D13" s="6">
-        <v>1.6546085392659901E-3</v>
+        <v>2.7043526110417599E-3</v>
       </c>
       <c r="E13" s="4">
         <v>60</v>
@@ -2380,13 +2380,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="2">
-        <v>1.97766017913818</v>
+        <v>2.5471699237823402</v>
       </c>
       <c r="C14" s="7">
-        <v>1.636347715122E-3</v>
+        <v>2.6707576171805399E-3</v>
       </c>
       <c r="D14" s="7">
-        <v>1.64580021420137E-3</v>
+        <v>2.6850770425764798E-3</v>
       </c>
       <c r="E14" s="2">
         <v>61</v>
@@ -2400,13 +2400,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="2">
-        <v>1.97766017913818</v>
+        <v>2.5471699237823402</v>
       </c>
       <c r="C15" s="7">
-        <v>1.6397932609543201E-3</v>
+        <v>2.6707805910458102E-3</v>
       </c>
       <c r="D15" s="7">
-        <v>1.64016782296227E-3</v>
+        <v>2.6697110151872E-3</v>
       </c>
       <c r="E15" s="2">
         <v>62</v>
@@ -2420,13 +2420,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="2">
-        <v>1.97766017913818</v>
+        <v>2.5471699237823402</v>
       </c>
       <c r="C16" s="7">
-        <v>1.6422623184819999E-3</v>
+        <v>2.6878361565371299E-3</v>
       </c>
       <c r="D16" s="7">
-        <v>1.6355306588786999E-3</v>
+        <v>2.6794429571228998E-3</v>
       </c>
       <c r="E16" s="2">
         <v>63</v>
@@ -2440,13 +2440,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="2">
-        <v>1.97766017913818</v>
+        <v>2.5471699237823402</v>
       </c>
       <c r="C17" s="7">
-        <v>1.6343076104919101E-3</v>
+        <v>2.66886778051654E-3</v>
       </c>
       <c r="D17" s="7">
-        <v>1.6461941834658E-3</v>
+        <v>2.68837927216465E-3</v>
       </c>
       <c r="E17" s="2">
         <v>64</v>
@@ -4230,7 +4230,7 @@
   <dimension ref="A1:N50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4278,10 +4278,10 @@
         <v>1E-8</v>
       </c>
       <c r="B2" s="7">
-        <v>1.6457066694274499E-3</v>
+        <v>2.6814372893422798E-3</v>
       </c>
       <c r="C2" s="7">
-        <v>1.6545231709197299E-3</v>
+        <v>2.6934186090774598E-3</v>
       </c>
       <c r="D2" s="2">
         <v>137</v>
@@ -4290,7 +4290,7 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>2.98</v>
+        <v>7.6509999999999998</v>
       </c>
       <c r="J2" s="5">
         <f ca="1">AVERAGE(OFFSET(A$2,(ROW()-2)*4,0,4,1))</f>
@@ -4298,11 +4298,11 @@
       </c>
       <c r="K2" s="6">
         <f t="shared" ref="K2:N9" ca="1" si="0">AVERAGE(OFFSET(B$2,(ROW()-2)*4,0,4,1))</f>
-        <v>1.6430723464582074E-3</v>
+        <v>2.6759812048015473E-3</v>
       </c>
       <c r="L2" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>1.6458375959042826E-3</v>
+        <v>2.6822605701609199E-3</v>
       </c>
       <c r="M2" s="5">
         <f t="shared" ca="1" si="0"/>
@@ -4318,10 +4318,10 @@
         <v>1E-8</v>
       </c>
       <c r="B3" s="7">
-        <v>1.6430577297384501E-3</v>
+        <v>2.6722184543808299E-3</v>
       </c>
       <c r="C3" s="7">
-        <v>1.64115236591587E-3</v>
+        <v>2.66995809060779E-3</v>
       </c>
       <c r="D3" s="2">
         <v>138</v>
@@ -4330,7 +4330,7 @@
         <v>1</v>
       </c>
       <c r="F3">
-        <v>5.6319999999999997</v>
+        <v>19.641999999999999</v>
       </c>
       <c r="J3" s="5">
         <f t="shared" ref="J3:J9" ca="1" si="1">AVERAGE(OFFSET(A$2,(ROW()-2)*4,0,4,1))</f>
@@ -4338,11 +4338,11 @@
       </c>
       <c r="K3" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>1.6448951116763025E-3</v>
+        <v>2.6806210184780227E-3</v>
       </c>
       <c r="L3" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>1.6470975131093598E-3</v>
+        <v>2.6851349239029503E-3</v>
       </c>
       <c r="M3" s="5">
         <f t="shared" ca="1" si="0"/>
@@ -4358,10 +4358,10 @@
         <v>1E-8</v>
       </c>
       <c r="B4" s="7">
-        <v>1.64205641858279E-3</v>
+        <v>2.6788104722897201E-3</v>
       </c>
       <c r="C4" s="7">
-        <v>1.6364359502442801E-3</v>
+        <v>2.6743481594553899E-3</v>
       </c>
       <c r="D4" s="2">
         <v>139</v>
@@ -4370,7 +4370,7 @@
         <v>1</v>
       </c>
       <c r="F4">
-        <v>7.3280000000000003</v>
+        <v>19.960999999999999</v>
       </c>
       <c r="J4" s="5">
         <f t="shared" ca="1" si="1"/>
@@ -4398,10 +4398,10 @@
         <v>1E-8</v>
       </c>
       <c r="B5" s="7">
-        <v>1.6414685680841399E-3</v>
+        <v>2.6714586031933601E-3</v>
       </c>
       <c r="C5" s="7">
-        <v>1.65123889653725E-3</v>
+        <v>2.6913174215030399E-3</v>
       </c>
       <c r="D5" s="2">
         <v>140</v>
@@ -4410,7 +4410,7 @@
         <v>1</v>
       </c>
       <c r="F5">
-        <v>3.6240000000000001</v>
+        <v>13.461</v>
       </c>
       <c r="J5" s="5">
         <f t="shared" ca="1" si="1"/>
@@ -4438,10 +4438,10 @@
         <v>9.9999999999999995E-8</v>
       </c>
       <c r="B6" s="6">
-        <v>1.64668200630694E-3</v>
+        <v>2.6842543501406899E-3</v>
       </c>
       <c r="C6" s="6">
-        <v>1.6553057815899301E-3</v>
+        <v>2.6946792483052298E-3</v>
       </c>
       <c r="D6" s="4">
         <v>141</v>
@@ -4476,10 +4476,10 @@
         <v>9.9999999999999995E-8</v>
       </c>
       <c r="B7" s="6">
-        <v>1.6449793176725499E-3</v>
+        <v>2.67692176438868E-3</v>
       </c>
       <c r="C7" s="6">
-        <v>1.64221417520472E-3</v>
+        <v>2.6730174010500601E-3</v>
       </c>
       <c r="D7" s="4">
         <v>142</v>
@@ -4514,10 +4514,10 @@
         <v>9.9999999999999995E-8</v>
       </c>
       <c r="B8" s="6">
-        <v>1.6442012668897699E-3</v>
+        <v>2.6820637304335801E-3</v>
       </c>
       <c r="C8" s="6">
-        <v>1.6382819504794099E-3</v>
+        <v>2.6769175446849799E-3</v>
       </c>
       <c r="D8" s="4">
         <v>143</v>
@@ -4552,10 +4552,10 @@
         <v>9.9999999999999995E-8</v>
       </c>
       <c r="B9" s="6">
-        <v>1.6437178558359499E-3</v>
+        <v>2.6792442289491399E-3</v>
       </c>
       <c r="C9" s="6">
-        <v>1.65258814516338E-3</v>
+        <v>2.69592550157153E-3</v>
       </c>
       <c r="D9" s="4">
         <v>144</v>

</xml_diff>